<commit_message>
fix(facilitator): redirect after payment
- Redirect to participants page after payment.
- Close create modal after redirect.
- Updated list styling in facilitator page.
</commit_message>
<xml_diff>
--- a/public/template-kolektif.xlsx
+++ b/public/template-kolektif.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\freelance\jcc\jcc-frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BBBABE-CCB0-46E0-BFA1-CF3AC69179AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4915E1-A633-4A9C-907E-8F873FC37CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{8CBE3E04-2605-47F7-8455-0CB910A98782}"/>
+    <workbookView xWindow="1815" yWindow="975" windowWidth="21600" windowHeight="11295" xr2:uid="{8CBE3E04-2605-47F7-8455-0CB910A98782}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -304,9 +304,6 @@
     <t>kelas</t>
   </si>
   <si>
-    <t>tangalLahir</t>
-  </si>
-  <si>
     <t>matpel</t>
   </si>
   <si>
@@ -332,6 +329,9 @@
   </si>
   <si>
     <t>Genteng</t>
+  </si>
+  <si>
+    <t>tanggalLahir</t>
   </si>
 </sst>
 </file>
@@ -412,10 +412,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -738,7 +734,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,21 +778,21 @@
         <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
       </c>
       <c r="K1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -808,7 +804,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -828,10 +824,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -843,7 +839,7 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
@@ -863,10 +859,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -878,7 +874,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>

</xml_diff>